<commit_message>
progress on google search
</commit_message>
<xml_diff>
--- a/intents.xlsx
+++ b/intents.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shacl\Documents\Best_Senior_Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED55AF8-C34A-4458-9F3E-719CB3FB409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7354DB34-C3ED-4332-9AEA-FFA5A1E51B35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A904A1FD-CE70-854E-8203-837AFAC8F14B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="102">
   <si>
     <t>get_weather</t>
   </si>
@@ -320,6 +320,27 @@
   </si>
   <si>
     <t>what day is today</t>
+  </si>
+  <si>
+    <t>cancel timer</t>
+  </si>
+  <si>
+    <t>cancel my timer</t>
+  </si>
+  <si>
+    <t>cancel my alarm</t>
+  </si>
+  <si>
+    <t>google_search</t>
+  </si>
+  <si>
+    <t>google search</t>
+  </si>
+  <si>
+    <t>search on google</t>
+  </si>
+  <si>
+    <t>look up</t>
   </si>
 </sst>
 </file>
@@ -674,10 +695,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A607722-EB0E-E340-AF2D-70550FC53A35}">
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -693,7 +714,7 @@
     <col min="9" max="9" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -721,8 +742,11 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -750,8 +774,11 @@
       <c r="I2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -776,8 +803,11 @@
       <c r="I3" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -799,8 +829,11 @@
       <c r="I4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -823,7 +856,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -846,7 +879,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -869,7 +902,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>15</v>
       </c>
@@ -889,7 +922,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -906,7 +939,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -916,11 +949,14 @@
       <c r="E10" t="s">
         <v>55</v>
       </c>
+      <c r="H10" t="s">
+        <v>97</v>
+      </c>
       <c r="I10" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>18</v>
       </c>
@@ -930,8 +966,11 @@
       <c r="E11" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>19</v>
       </c>
@@ -941,8 +980,11 @@
       <c r="E12" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>20</v>
       </c>
@@ -953,7 +995,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>21</v>
       </c>
@@ -964,7 +1006,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -975,7 +1017,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>23</v>
       </c>

</xml_diff>